<commit_message>
database and tables created
</commit_message>
<xml_diff>
--- a/carbon_cutdata.xlsx
+++ b/carbon_cutdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ForrestV\Documents\python\laserQuote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B22B7E-1901-496F-B13A-9A92BDDF628C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FE9630-1D5F-40F4-8260-FFAC636469CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31530" yWindow="825" windowWidth="24315" windowHeight="15375" xr2:uid="{195FF174-2A6F-4BE5-A905-02E9184E94C4}"/>
+    <workbookView xWindow="29190" yWindow="390" windowWidth="24315" windowHeight="15375" xr2:uid="{195FF174-2A6F-4BE5-A905-02E9184E94C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>CARBON STEEL</t>
-  </si>
-  <si>
     <t>0.035 [20GA]</t>
   </si>
   <si>
@@ -60,19 +57,22 @@
     <t>0.500 [HRPO]</t>
   </si>
   <si>
-    <t>COST PER SQUARE FOOT</t>
-  </si>
-  <si>
-    <t>CUT SPEED</t>
-  </si>
-  <si>
-    <t>PIERCE TIME</t>
-  </si>
-  <si>
     <t>WEIGHT</t>
   </si>
   <si>
-    <t>MATERIAL COST</t>
+    <t>CARBON_STEEL</t>
+  </si>
+  <si>
+    <t>CUT_SPEED</t>
+  </si>
+  <si>
+    <t>PIERCE_TIME</t>
+  </si>
+  <si>
+    <t>MATERIAL_COST</t>
+  </si>
+  <si>
+    <t>COST_SQUARE_FOOT</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:F19"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -453,18 +453,18 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>160</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>140</v>
@@ -500,13 +500,13 @@
         <v>0.9</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F19" si="0">D3*E3</f>
+        <f t="shared" ref="F3:F11" si="0">D3*E3</f>
         <v>1.764</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>115</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>85</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>80</v>
@@ -590,7 +590,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>55</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>25</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>16</v>

</xml_diff>

<commit_message>
select certain item from database and enter to variable
</commit_message>
<xml_diff>
--- a/carbon_cutdata.xlsx
+++ b/carbon_cutdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ForrestV\Documents\python\laserQuote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FE9630-1D5F-40F4-8260-FFAC636469CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9017BF03-50ED-4F6A-9B42-B76D9C307075}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="390" windowWidth="24315" windowHeight="15375" xr2:uid="{195FF174-2A6F-4BE5-A905-02E9184E94C4}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="24315" windowHeight="15375" xr2:uid="{195FF174-2A6F-4BE5-A905-02E9184E94C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>WEIGHT</t>
   </si>
   <si>
-    <t>CARBON_STEEL</t>
-  </si>
-  <si>
     <t>CUT_SPEED</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>COST_SQUARE_FOOT</t>
+  </si>
+  <si>
+    <t>STEEL</t>
   </si>
 </sst>
 </file>
@@ -426,9 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602AB0E5-F549-4D47-8A56-90431E725018}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -444,22 +442,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
one table with carbon and stainless in it.  Can retrieve data now
</commit_message>
<xml_diff>
--- a/carbon_cutdata.xlsx
+++ b/carbon_cutdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ForrestV\Documents\python\laserQuote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9017BF03-50ED-4F6A-9B42-B76D9C307075}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CEE54B-CC34-4CCC-BE48-5741CF8BEBD5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="24315" windowHeight="15375" xr2:uid="{195FF174-2A6F-4BE5-A905-02E9184E94C4}"/>
+    <workbookView xWindow="29970" yWindow="825" windowWidth="24315" windowHeight="15375" xr2:uid="{195FF174-2A6F-4BE5-A905-02E9184E94C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,37 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>0.035 [20GA]</t>
-  </si>
-  <si>
-    <t>0.047 [18GA]</t>
-  </si>
-  <si>
-    <t>0.060 [16GA]</t>
-  </si>
-  <si>
-    <t>0.075 [14GA]</t>
-  </si>
-  <si>
-    <t>0.105 [12GA]</t>
-  </si>
-  <si>
-    <t>0.120 [11GA]</t>
-  </si>
-  <si>
-    <t>0.187 [HRPO]</t>
-  </si>
-  <si>
-    <t>0.250 [HRPO]</t>
-  </si>
-  <si>
-    <t>0.375 [HRPO]</t>
-  </si>
-  <si>
-    <t>0.500 [HRPO]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>WEIGHT</t>
   </si>
@@ -79,6 +49,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -108,8 +81,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,9 +399,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602AB0E5-F549-4D47-8A56-90431E725018}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -442,27 +419,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2" s="2">
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="B2">
         <v>160</v>
@@ -470,20 +447,20 @@
       <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <f>D2*E2</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="A3" s="2">
+        <v>4.7E-2</v>
       </c>
       <c r="B3">
         <v>140</v>
@@ -491,20 +468,20 @@
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1.96</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>0.9</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <f t="shared" ref="F3:F11" si="0">D3*E3</f>
         <v>1.764</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
+      <c r="A4" s="2">
+        <v>0.06</v>
       </c>
       <c r="B4">
         <v>115</v>
@@ -512,20 +489,20 @@
       <c r="C4">
         <v>5.5</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>2.65</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>0.75</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <f t="shared" si="0"/>
         <v>1.9874999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="A5" s="2">
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -533,20 +510,20 @@
       <c r="C5">
         <v>7.5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>3.06</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>0.75</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <f t="shared" si="0"/>
         <v>2.2949999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
+      <c r="A6" s="2">
+        <v>0.105</v>
       </c>
       <c r="B6">
         <v>85</v>
@@ -554,20 +531,20 @@
       <c r="C6">
         <v>9.5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>4.375</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>0.75</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <f t="shared" si="0"/>
         <v>3.28125</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
+      <c r="A7" s="2">
+        <v>0.12</v>
       </c>
       <c r="B7">
         <v>80</v>
@@ -575,20 +552,20 @@
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>0.75</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
+      <c r="A8" s="2">
+        <v>0.187</v>
       </c>
       <c r="B8">
         <v>55</v>
@@ -596,20 +573,20 @@
       <c r="C8">
         <v>8</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>7.66</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>0.76</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
         <v>5.8216000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
+      <c r="A9" s="2">
+        <v>0.25</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -617,20 +594,20 @@
       <c r="C9">
         <v>10</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>10.210000000000001</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>0.77</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <f t="shared" si="0"/>
         <v>7.8617000000000008</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
+      <c r="A10" s="2">
+        <v>0.375</v>
       </c>
       <c r="B10">
         <v>25</v>
@@ -638,20 +615,20 @@
       <c r="C10">
         <v>30</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>15.31</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>0.9</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <f t="shared" si="0"/>
         <v>13.779</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
+      <c r="A11" s="2">
+        <v>0.5</v>
       </c>
       <c r="B11">
         <v>16</v>
@@ -659,16 +636,22 @@
       <c r="C11">
         <v>33</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>20.420000000000002</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>0.92</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <f t="shared" si="0"/>
         <v>18.786400000000004</v>
       </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>